<commit_message>
Update Pytest capture folder cont'
</commit_message>
<xml_diff>
--- a/diagram.xlsx
+++ b/diagram.xlsx
@@ -67,6 +67,64 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rounded Rectangle 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="247649"/>
+          <a:ext cx="8782050" cy="4362451"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Project root directory</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304799</xdr:colOff>
       <xdr:row>26</xdr:row>
@@ -125,14 +183,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>542924</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>428624</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -142,67 +200,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2867024" y="895350"/>
-          <a:ext cx="1828800" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1050"/>
-            <a:t>pysniff</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rounded Rectangle 3"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="904874" y="2133600"/>
+          <a:off x="2981324" y="361950"/>
           <a:ext cx="2743200" cy="1828800"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -235,49 +233,11 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1000" b="1"/>
-            <a:t>.gitignore</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="1"/>
-            <a:t>-----------------------------------</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" baseline="0"/>
-            <a:t>C</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000"/>
-            <a:t>ontent which not sync up </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" baseline="0"/>
-            <a:t>in git</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
+            <a:t>pysniff</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1000" b="1">
               <a:solidFill>
@@ -288,61 +248,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>-----------------------------------</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>File</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1000" b="0">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1000"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
+            <a:t>-------------------------------------------------------</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1000"/>
         </a:p>
       </xdr:txBody>
@@ -351,26 +258,26 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>485774</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>485774</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rounded Rectangle 4"/>
+        <xdr:cNvPr id="4" name="Rounded Rectangle 3"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5362574" y="2181225"/>
-          <a:ext cx="1828800" cy="914400"/>
+          <a:off x="800099" y="2562225"/>
+          <a:ext cx="2743200" cy="1828800"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -401,32 +308,302 @@
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:rPr lang="en-US" sz="1000" b="1"/>
+            <a:t>.gitignore</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="1"/>
+            <a:t>------------------------------------------------------------</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t>C</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>ontent which not sync up </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t>in git</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>-------------------------------------------------------</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="1">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Unversioned</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> file;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Log directory</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Capture direcetory if there is any big size capture files</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="0">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1000"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rounded Rectangle 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5295899" y="2476500"/>
+          <a:ext cx="2743200" cy="1828800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="1"/>
             <a:t>config.ini</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>-------------------------------------------------------</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="1"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
             <a:t>- basic config</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>-------------------------------------------------------</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
             <a:t>-</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
             <a:t> D</a:t>
           </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+          <a:endParaRPr lang="en-US" sz="1000"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1000"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -725,7 +902,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>